<commit_message>
finished up to and including part 7
</commit_message>
<xml_diff>
--- a/Code/DAV Proforma Acc Analy.xlsx
+++ b/Code/DAV Proforma Acc Analy.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DAV Proforma Acc Analy" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -445,7 +445,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Periodicity:</t>
+          <t>Periodicity</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">

</xml_diff>